<commit_message>
correct smoking frequency recode to be consistent with other studies
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atrottier\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBBA7A4-A8F7-4F00-8247-670E38058E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19596889-6A1A-4C14-8DA7-95124F6C9299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1079,9 +1079,6 @@
     <t>recode(1=2; 2=2; 3=2; 4=1; 5=0; ELSE=NA)</t>
   </si>
   <si>
-    <t>recode(1=2; 2=1; 3=1; 4=NA; 5=NA; ELSE=NA)</t>
-  </si>
-  <si>
     <t>as.numeric(sp28a) * 7</t>
   </si>
   <si>
@@ -1104,6 +1101,9 @@
   </si>
   <si>
     <t>recode(3=0; 2=1; 1=1; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>recode(1=2; 2=NA; 3=1; 4=NA; 5=NA; ELSE=NA)</t>
   </si>
 </sst>
 </file>
@@ -1561,10 +1561,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2:S84"/>
+      <selection pane="bottomRight" activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3629,7 +3629,7 @@
         <v>33</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -3676,7 +3676,7 @@
         <v>29</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
@@ -4142,7 +4142,7 @@
       </c>
       <c r="L58" s="3"/>
       <c r="M58" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="L69" s="3"/>
       <c r="M69" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
@@ -4619,7 +4619,7 @@
         <v>33</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="51" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
correct vegetables and fruit veluetype
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19596889-6A1A-4C14-8DA7-95124F6C9299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E764774-F8C0-4E9B-8E11-0B72B9131C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -1242,7 +1242,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1561,13 +1561,13 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S46" sqref="S46"/>
+      <selection pane="bottomRight" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="2" customWidth="1"/>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>120</v>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
correcting bmi and harmo status details
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBF2AA3-67BE-428B-A705-1BE36D5B8CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE52659-82FA-4D26-AB40-0311EFE73539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1774,10 +1774,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T7" sqref="T7"/>
+      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,7 +1801,7 @@
     <col min="17" max="17" width="12.42578125" style="2" customWidth="1"/>
     <col min="18" max="18" width="17.5703125" style="2" customWidth="1"/>
     <col min="19" max="19" width="19.85546875" style="2" customWidth="1"/>
-    <col min="23" max="23" width="29.42578125" customWidth="1"/>
+    <col min="23" max="23" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -2678,7 +2678,7 @@
         <v>22</v>
       </c>
       <c r="U16" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="V16" t="s">
         <v>29</v>
@@ -2789,7 +2789,7 @@
         <v>22</v>
       </c>
       <c r="U18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="V18" t="s">
         <v>29</v>
@@ -2900,10 +2900,10 @@
         <v>22</v>
       </c>
       <c r="U20" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="V20" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="W20" t="s">
         <v>329</v>
@@ -3886,7 +3886,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="180" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Correction as.numeric harmo rule to avoid warning coercion to NA
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE52659-82FA-4D26-AB40-0311EFE73539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E30ECB3-D596-4844-8271-B903E404DB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -893,9 +893,6 @@
     <t>recode(1=2; 2=2; 3=2; 4=1; 5=0; ELSE=NA)</t>
   </si>
   <si>
-    <t>as.numeric(sp28a) * 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 Excellent
 2 Very good
 3 Good
@@ -920,9 +917,6 @@
     <t>recode(1=2; 2=NA; 3=1; 4=NA; 5=NA; ELSE=NA)</t>
   </si>
   <si>
-    <t>as.numeric(drukuge2)*12</t>
-  </si>
-  <si>
     <t>Construct label</t>
   </si>
   <si>
@@ -1072,16 +1066,10 @@
 2 = Urban</t>
   </si>
   <si>
-    <t>as.numeric(sp58)</t>
-  </si>
-  <si>
     <t>1 = Self-reported ; 
 2 = Measured by professional</t>
   </si>
   <si>
-    <t>ifelse(!is.na(as.numeric(sp58)), 1, NA)</t>
-  </si>
-  <si>
     <t>need to confirm if it is measured by a profesional or self measured (for now professional)</t>
   </si>
   <si>
@@ -1089,15 +1077,6 @@
   </si>
   <si>
     <t>Self-reported</t>
-  </si>
-  <si>
-    <t>as.numeric(sp59)</t>
-  </si>
-  <si>
-    <t>ifelse(!is.na(as.numeric(sp59)), 1, NA)</t>
-  </si>
-  <si>
-    <t>as.numeric(bmi)</t>
   </si>
   <si>
     <t>Systolic blood pressure, average of all measures available</t>
@@ -1314,6 +1293,27 @@
   </si>
   <si>
     <t>Number of non-missing items in the SF36 physical function subscale</t>
+  </si>
+  <si>
+    <t>ifelse(sp58 %in% c("Uoplyst","."),NA,sp58)</t>
+  </si>
+  <si>
+    <t>ifelse(sp58 %in% c("Uoplyst","."),NA,1)</t>
+  </si>
+  <si>
+    <t>ifelse(sp59 %in% c("Uoplyst","."),NA,sp59)</t>
+  </si>
+  <si>
+    <t>ifelse(sp59 %in% c("Uoplyst","."),NA,1)</t>
+  </si>
+  <si>
+    <t>ifelse(drukuge2 %in% c("Uoplyst",".","Irrelevant"),NA,drukuge2*12)</t>
+  </si>
+  <si>
+    <t>ifelse(bmi %in% c("Uoplyst",".",".u"),NA,bmi)</t>
+  </si>
+  <si>
+    <t>ifelse(sp28a %in% c("Uoplyst",".","Irrelevant"),NA,sp28a*7)</t>
   </si>
 </sst>
 </file>
@@ -1774,10 +1774,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
+      <selection pane="bottomRight" activeCell="W46" sqref="W46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,19 +1839,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>279</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>281</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>12</v>
@@ -1875,25 +1875,25 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
+        <v>280</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z1" t="s">
         <v>282</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>283</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>284</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>285</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>286</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>287</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>21</v>
@@ -1945,7 +1945,7 @@
         <v>223</v>
       </c>
       <c r="Y2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -1962,7 +1962,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>27</v>
@@ -2011,7 +2011,7 @@
         <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>32</v>
@@ -2019,7 +2019,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>225</v>
@@ -2064,7 +2064,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>32</v>
@@ -2103,10 +2103,10 @@
         <v>37</v>
       </c>
       <c r="Y5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AA5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="199.5" x14ac:dyDescent="0.25">
@@ -2123,7 +2123,7 @@
         <v>39</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>32</v>
@@ -2131,7 +2131,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>229</v>
@@ -2162,7 +2162,7 @@
         <v>46</v>
       </c>
       <c r="X6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="270" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>32</v>
@@ -2187,7 +2187,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>231</v>
@@ -2215,7 +2215,7 @@
         <v>260</v>
       </c>
       <c r="X7" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="213.75" x14ac:dyDescent="0.25">
@@ -2232,7 +2232,7 @@
         <v>45</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>32</v>
@@ -2240,7 +2240,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>232</v>
@@ -2271,10 +2271,10 @@
         <v>262</v>
       </c>
       <c r="AA8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AB8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2291,7 +2291,7 @@
         <v>49</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>32</v>
@@ -2299,7 +2299,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>43</v>
@@ -2340,7 +2340,7 @@
         <v>51</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>52</v>
@@ -2387,7 +2387,7 @@
         <v>54</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>21</v>
@@ -2434,7 +2434,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>32</v>
@@ -2442,7 +2442,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>232</v>
@@ -2473,10 +2473,10 @@
         <v>263</v>
       </c>
       <c r="AA12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AB12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>58</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>32</v>
@@ -2501,7 +2501,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>234</v>
@@ -2532,10 +2532,10 @@
         <v>265</v>
       </c>
       <c r="Y13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AA13" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2552,7 +2552,7 @@
         <v>60</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>32</v>
@@ -2560,7 +2560,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>43</v>
@@ -2609,7 +2609,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>43</v>
@@ -2684,7 +2684,7 @@
         <v>29</v>
       </c>
       <c r="W16" t="s">
-        <v>321</v>
+        <v>374</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
@@ -2709,7 +2709,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>236</v>
@@ -2735,16 +2735,16 @@
         <v>29</v>
       </c>
       <c r="W17" t="s">
-        <v>323</v>
+        <v>375</v>
       </c>
       <c r="X17" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="Y17" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="AA17" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
@@ -2795,7 +2795,7 @@
         <v>29</v>
       </c>
       <c r="W18" t="s">
-        <v>327</v>
+        <v>376</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
@@ -2820,7 +2820,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>238</v>
@@ -2846,16 +2846,16 @@
         <v>29</v>
       </c>
       <c r="W19" t="s">
-        <v>328</v>
+        <v>377</v>
       </c>
       <c r="X19" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="Y19" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="AA19" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
@@ -2906,7 +2906,7 @@
         <v>29</v>
       </c>
       <c r="W20" t="s">
-        <v>329</v>
+        <v>379</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>43</v>
@@ -3113,7 +3113,7 @@
         <v>86</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>32</v>
@@ -3162,7 +3162,7 @@
         <v>89</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>32</v>
@@ -3317,7 +3317,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="8" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="J29" s="11" t="s">
         <v>43</v>
@@ -3750,7 +3750,7 @@
         <v>119</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>52</v>
@@ -3799,7 +3799,7 @@
         <v>123</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>32</v>
@@ -3807,7 +3807,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="8" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="J39" s="11" t="s">
         <v>241</v>
@@ -3852,7 +3852,7 @@
         <v>125</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>52</v>
@@ -3886,7 +3886,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="180" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="171" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>127</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>32</v>
@@ -3908,13 +3908,13 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="8" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="8"/>
@@ -3936,7 +3936,7 @@
         <v>159</v>
       </c>
       <c r="W41" s="13" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
@@ -4002,7 +4002,7 @@
         <v>132</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>52</v>
@@ -4036,16 +4036,16 @@
         <v>29</v>
       </c>
       <c r="W43" t="s">
-        <v>277</v>
+        <v>378</v>
       </c>
       <c r="Y43" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="AA43" s="13" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="AB43" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:28" ht="51" x14ac:dyDescent="0.25">
@@ -4070,7 +4070,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="8" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="J44" s="11" t="s">
         <v>43</v>
@@ -4111,7 +4111,7 @@
         <v>137</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>32</v>
@@ -4119,7 +4119,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="8" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="J45" s="11" t="s">
         <v>245</v>
@@ -4172,7 +4172,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="8" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="J46" s="11" t="s">
         <v>245</v>
@@ -4200,7 +4200,7 @@
         <v>33</v>
       </c>
       <c r="W46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
         <v>29</v>
       </c>
       <c r="W47" t="s">
-        <v>271</v>
+        <v>380</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="99.75" x14ac:dyDescent="0.25">
@@ -4278,7 +4278,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="8" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="J48" s="11" t="s">
         <v>249</v>
@@ -4292,7 +4292,7 @@
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
@@ -4323,7 +4323,7 @@
         <v>146</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>32</v>
@@ -4331,7 +4331,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J49" s="11" t="s">
         <v>43</v>
@@ -4371,7 +4371,7 @@
         <v>148</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>32</v>
@@ -4379,7 +4379,7 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>43</v>
@@ -4428,7 +4428,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J51" s="11" t="s">
         <v>43</v>
@@ -4477,7 +4477,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="8" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="J52" s="11" t="s">
         <v>43</v>
@@ -4526,7 +4526,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J53" s="11" t="s">
         <v>43</v>
@@ -4575,7 +4575,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J54" s="11" t="s">
         <v>43</v>
@@ -4624,7 +4624,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J55" s="11" t="s">
         <v>43</v>
@@ -4651,10 +4651,10 @@
         <v>46</v>
       </c>
       <c r="AA55" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="AB55" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="56" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
@@ -4679,7 +4679,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J56" s="11" t="s">
         <v>43</v>
@@ -4728,7 +4728,7 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J57" s="11" t="s">
         <v>43</v>
@@ -4755,10 +4755,10 @@
         <v>46</v>
       </c>
       <c r="AA57" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="AB57" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="58" spans="1:28" ht="28.5" x14ac:dyDescent="0.25">
@@ -4775,7 +4775,7 @@
         <v>165</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>32</v>
@@ -4783,7 +4783,7 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J58" s="11" t="s">
         <v>251</v>
@@ -4797,7 +4797,7 @@
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
       <c r="Q58" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
@@ -4814,10 +4814,10 @@
         <v>46</v>
       </c>
       <c r="Y58" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="AA58" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.25">
@@ -5171,7 +5171,7 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="8" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="J66" s="11" t="s">
         <v>43</v>
@@ -5269,7 +5269,7 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="8" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="J68" s="11" t="s">
         <v>43</v>
@@ -5318,7 +5318,7 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="8" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="J69" s="11" t="s">
         <v>252</v>
@@ -5332,7 +5332,7 @@
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R69" s="3"/>
       <c r="S69" s="3"/>
@@ -5346,7 +5346,7 @@
         <v>33</v>
       </c>
       <c r="W69" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="70" spans="1:24" ht="51" x14ac:dyDescent="0.25">
@@ -5371,7 +5371,7 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="8" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="J70" s="11" t="s">
         <v>43</v>
@@ -5420,7 +5420,7 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="8" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="J71" s="11" t="s">
         <v>43</v>
@@ -5469,7 +5469,7 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="8" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="J72" s="11" t="s">
         <v>43</v>
@@ -5510,7 +5510,7 @@
         <v>196</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>32</v>
@@ -5518,7 +5518,7 @@
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="8" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="J73" s="11" t="s">
         <v>43</v>
@@ -5559,7 +5559,7 @@
         <v>198</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>32</v>
@@ -5567,7 +5567,7 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="8" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="J74" s="11" t="s">
         <v>43</v>
@@ -5608,7 +5608,7 @@
         <v>200</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>32</v>
@@ -5616,7 +5616,7 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="8" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="J75" s="11" t="s">
         <v>43</v>
@@ -5657,7 +5657,7 @@
         <v>202</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>32</v>
@@ -5706,14 +5706,14 @@
         <v>204</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G77" s="3"/>
       <c r="I77" s="9" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="J77" s="11" t="s">
         <v>43</v>
@@ -5754,7 +5754,7 @@
         <v>206</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>32</v>
@@ -5762,7 +5762,7 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="8" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="J78" s="11" t="s">
         <v>43</v>
@@ -5811,7 +5811,7 @@
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="8" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="J79" s="11" t="s">
         <v>43</v>
@@ -5838,7 +5838,7 @@
         <v>46</v>
       </c>
       <c r="X79" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="80" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -5855,7 +5855,7 @@
         <v>210</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>32</v>
@@ -5863,7 +5863,7 @@
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J80" s="11" t="s">
         <v>43</v>
@@ -5904,7 +5904,7 @@
         <v>212</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>32</v>
@@ -5912,7 +5912,7 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J81" s="11" t="s">
         <v>43</v>
@@ -5953,7 +5953,7 @@
         <v>214</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>32</v>
@@ -5961,7 +5961,7 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J82" s="11" t="s">
         <v>43</v>
@@ -5990,10 +5990,10 @@
         <v>46</v>
       </c>
       <c r="X82" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="AA82" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.25">
@@ -6010,7 +6010,7 @@
         <v>216</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>32</v>
@@ -6057,7 +6057,7 @@
         <v>218</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Correct bmi, drukuge2 and sp28a
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E30ECB3-D596-4844-8271-B903E404DB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E148FA3F-5364-4840-AA61-F8B7FFE3A6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1307,13 +1307,13 @@
     <t>ifelse(sp59 %in% c("Uoplyst","."),NA,1)</t>
   </si>
   <si>
-    <t>ifelse(drukuge2 %in% c("Uoplyst",".","Irrelevant"),NA,drukuge2*12)</t>
-  </si>
-  <si>
-    <t>ifelse(bmi %in% c("Uoplyst",".",".u"),NA,bmi)</t>
-  </si>
-  <si>
-    <t>ifelse(sp28a %in% c("Uoplyst",".","Irrelevant"),NA,sp28a*7)</t>
+    <t>ifelse(sp28a %in% c("Uoplyst",".","Irrelevant",NA),NA,sp28a*7)</t>
+  </si>
+  <si>
+    <t>ifelse(drukuge2 %in% c(NA,"Uoplyst",".","Irrelevant"),NA,drukuge2*12)</t>
+  </si>
+  <si>
+    <t>ifelse(bmi %in% c(NA,"Uoplyst",".",".u"),NA,bmi)</t>
   </si>
 </sst>
 </file>
@@ -1774,10 +1774,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W46" sqref="W46"/>
+      <selection pane="bottomRight" activeCell="X46" sqref="X46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,7 +2906,7 @@
         <v>29</v>
       </c>
       <c r="W20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
@@ -4036,7 +4036,7 @@
         <v>29</v>
       </c>
       <c r="W43" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="Y43" t="s">
         <v>335</v>
@@ -4253,7 +4253,7 @@
         <v>29</v>
       </c>
       <c r="W47" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="99.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
same as the one before
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E148FA3F-5364-4840-AA61-F8B7FFE3A6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7A8073-6CAE-423B-9FFF-35F5581FA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1307,13 +1307,13 @@
     <t>ifelse(sp59 %in% c("Uoplyst","."),NA,1)</t>
   </si>
   <si>
-    <t>ifelse(sp28a %in% c("Uoplyst",".","Irrelevant",NA),NA,sp28a*7)</t>
-  </si>
-  <si>
-    <t>ifelse(drukuge2 %in% c(NA,"Uoplyst",".","Irrelevant"),NA,drukuge2*12)</t>
-  </si>
-  <si>
-    <t>ifelse(bmi %in% c(NA,"Uoplyst",".",".u"),NA,bmi)</t>
+    <t>ifelse(drukuge2 %in% c("NA","Uoplyst",".","Irrelevant"),NA,drukuge2*12)</t>
+  </si>
+  <si>
+    <t>ifelse(sp28a %in% c("Uoplyst",".","Irrelevant","NA"),NA,sp28a*7)</t>
+  </si>
+  <si>
+    <t>ifelse(bmi %in% c("NA","Uoplyst",".",".u"),NA,bmi)</t>
   </si>
 </sst>
 </file>
@@ -1774,10 +1774,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X46" sqref="X46"/>
+      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4036,7 +4036,7 @@
         <v>29</v>
       </c>
       <c r="W43" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Y43" t="s">
         <v>335</v>
@@ -4253,7 +4253,7 @@
         <v>29</v>
       </c>
       <c r="W47" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="99.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
explicit is.na for bmi, cigarettes and alcohol
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7A8073-6CAE-423B-9FFF-35F5581FA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99993D56-BCAD-4EC5-8AF7-132C9641267E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1307,13 +1307,13 @@
     <t>ifelse(sp59 %in% c("Uoplyst","."),NA,1)</t>
   </si>
   <si>
-    <t>ifelse(drukuge2 %in% c("NA","Uoplyst",".","Irrelevant"),NA,drukuge2*12)</t>
-  </si>
-  <si>
-    <t>ifelse(sp28a %in% c("Uoplyst",".","Irrelevant","NA"),NA,sp28a*7)</t>
-  </si>
-  <si>
-    <t>ifelse(bmi %in% c("NA","Uoplyst",".",".u"),NA,bmi)</t>
+    <t>ifelse(is.na(bmi) | bmi %in% c(,"Uoplyst",".",".u"),NA,bmi)</t>
+  </si>
+  <si>
+    <t>ifelse(is.na(drukuge2) | drukuge2 %in% c("Uoplyst",".","Irrelevant"),NA,drukuge2*12)</t>
+  </si>
+  <si>
+    <t>ifelse(is.na(sp28a) | sp28a %in% c("Uoplyst",".","Irrelevant"),NA,sp28a*7)</t>
   </si>
 </sst>
 </file>
@@ -1777,7 +1777,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="J13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
+      <selection pane="bottomRight" activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,7 +2906,7 @@
         <v>29</v>
       </c>
       <c r="W20" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
@@ -4036,7 +4036,7 @@
         <v>29</v>
       </c>
       <c r="W43" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="Y43" t="s">
         <v>335</v>
@@ -4253,7 +4253,7 @@
         <v>29</v>
       </c>
       <c r="W47" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="99.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correct all recodes and case_when
data contained the coding label and not the codes
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6993AC8-2D52-483F-ABB6-48D748025A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9FA8E8-0C19-4A03-BC72-D25922AC7553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -701,9 +701,6 @@
     <t>items</t>
   </si>
   <si>
-    <t>recode(1=4; 2=4; 3=3; 4=2; 5=1; ELSE=NA)</t>
-  </si>
-  <si>
     <t>cig/day</t>
   </si>
   <si>
@@ -808,9 +805,6 @@
   </si>
   <si>
     <t>2 = Female; 1 = Male</t>
-  </si>
-  <si>
-    <t>recode(1=2;2=1;ELSE=NA)</t>
   </si>
   <si>
     <t>Age is recorded at the time of invitation of participants on Jan. 1st 2023</t>
@@ -832,9 +826,6 @@
 </t>
   </si>
   <si>
-    <t>recode(1=1; 2=1; 3=NA; ELSE=NA)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1=Employed
 2=Unemployed
 3=Student
@@ -843,12 +834,6 @@
 6=Retiree
 7=Others outside the working-force
 </t>
-  </si>
-  <si>
-    <t>recode(1=1;2=0;3=NA;4=0;5=0;6=0;7=0;ELSE=NA)</t>
-  </si>
-  <si>
-    <t>recode(1=0;2=0;3=0;4=0;5=1;6=1;7=0;ELSE=NA)</t>
   </si>
   <si>
     <t>"Divorced"
@@ -872,9 +857,6 @@
 </t>
   </si>
   <si>
-    <t>recode(1=3; 2=3; 3=3; 4=3; 5=2; 6=2; 7=1; 8=1; ELSE=NA)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 More than once a day
 2 5-7 times a week
 3 3-4 times a week
@@ -890,9 +872,6 @@
 5 No, I have never smoked</t>
   </si>
   <si>
-    <t>recode(1=2; 2=2; 3=2; 4=1; 5=0; ELSE=NA)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 Excellent
 2 Very good
 3 Good
@@ -909,12 +888,6 @@
 2 Yes, slightly troubled
 3 No
 </t>
-  </si>
-  <si>
-    <t>recode(3=0; 2=1; 1=1; ELSE=NA)</t>
-  </si>
-  <si>
-    <t>recode(1=2; 2=NA; 3=1; 4=NA; 5=NA; ELSE=NA)</t>
   </si>
   <si>
     <t>Construct label</t>
@@ -1295,18 +1268,6 @@
     <t>Number of non-missing items in the SF36 physical function subscale</t>
   </si>
   <si>
-    <t>ifelse(sp58 %in% c("Uoplyst","."),NA,sp58)</t>
-  </si>
-  <si>
-    <t>ifelse(sp58 %in% c("Uoplyst","."),NA,1)</t>
-  </si>
-  <si>
-    <t>ifelse(sp59 %in% c("Uoplyst","."),NA,sp59)</t>
-  </si>
-  <si>
-    <t>ifelse(sp59 %in% c("Uoplyst","."),NA,1)</t>
-  </si>
-  <si>
     <t>as.numeric(bmi)</t>
   </si>
   <si>
@@ -1314,6 +1275,45 @@
   </si>
   <si>
     <t>as.numeric(sp28a)*7</t>
+  </si>
+  <si>
+    <t>recode("Danish ethnicity"=1; "Western ethnicity" =1; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>recode("Male"=2;"Female"=1;ELSE=NA)</t>
+  </si>
+  <si>
+    <t>recode("Employed"=1;"Unemployed"=0;"Student"=NA;"Disability pensioner"=0;"Early retiree"=0;"Retiree"=0;"Others outside the working-force"=0;ELSE=NA)</t>
+  </si>
+  <si>
+    <t>recode("Employed"=0;"Unemployed"=0;"Student"=0;"Disability pensioner"=0;"Early retiree"=1;"Retiree"=1;"Others outside the working-force"=0;ELSE=NA)</t>
+  </si>
+  <si>
+    <t>ifelse(sp58 %in% c("Uoplyst",".") | is.na(sp58),NA,sp58)</t>
+  </si>
+  <si>
+    <t>ifelse(sp58 %in% c("Uoplyst",".") | is.na(sp58),NA,1)</t>
+  </si>
+  <si>
+    <t>ifelse(sp59 %in% c("Uoplyst",".") | is.na(sp59),NA,sp59)</t>
+  </si>
+  <si>
+    <t>ifelse(sp59 %in% c("Uoplyst",".") | is.na(sp59),NA,1)</t>
+  </si>
+  <si>
+    <t>recode("More than 6 a day"=3; "5-6 per day"=3; "3-4 per day"=3; "1-2 per day"=3; "5-6 per week"=2; "3-4 per week"=2; "1-2 per week"=1; "None"=1; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>recode("Yes, every day"=2; "Yes, a least once a week"=2; "Yes, but less frequently than once a week"=2; "No, I've quit"=1; "No, I have never smoked"=0; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>recode("Yes, every day"=2; "Yes, a least once a week"=NA; "Yes, but less frequently than once a week"=1; "No, I've quit"=NA; "No, I have never smoked"=NA; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>recode("Excellent"=4; "Very good"=4; "Good"=3; "Less than good"=2; "Poor"=1; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>recode("No"=0; "Yes, slightly troubled"=1; "Yes, very troubled"=1; ELSE=NA)</t>
   </si>
 </sst>
 </file>
@@ -1774,10 +1774,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
+      <selection pane="bottomRight" activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,19 +1839,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>12</v>
@@ -1875,25 +1875,25 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="Y1" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="Z1" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="AA1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="AB1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="AC1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="AD1" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -1901,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>19</v>
@@ -1910,7 +1910,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>21</v>
@@ -1919,10 +1919,10 @@
       <c r="H2" s="3"/>
       <c r="I2" s="8"/>
       <c r="J2" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>224</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="8"/>
@@ -1942,10 +1942,10 @@
         <v>24</v>
       </c>
       <c r="W2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y2" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -1953,7 +1953,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>25</v>
@@ -1962,7 +1962,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>27</v>
@@ -2002,7 +2002,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>30</v>
@@ -2011,7 +2011,7 @@
         <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>32</v>
@@ -2019,13 +2019,13 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="8" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="J4" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="8"/>
@@ -2033,7 +2033,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
@@ -2047,7 +2047,7 @@
         <v>33</v>
       </c>
       <c r="W4" t="s">
-        <v>256</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>34</v>
@@ -2064,7 +2064,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>32</v>
@@ -2075,10 +2075,10 @@
       <c r="H5" s="3"/>
       <c r="I5" s="8"/>
       <c r="J5" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="8"/>
@@ -2088,7 +2088,7 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="T5" t="s">
         <v>22</v>
@@ -2103,10 +2103,10 @@
         <v>37</v>
       </c>
       <c r="Y5" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="AA5" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="199.5" x14ac:dyDescent="0.25">
@@ -2114,7 +2114,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>38</v>
@@ -2123,7 +2123,7 @@
         <v>39</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>32</v>
@@ -2131,13 +2131,13 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="8" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="J6" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="8"/>
@@ -2145,7 +2145,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
@@ -2162,7 +2162,7 @@
         <v>46</v>
       </c>
       <c r="X6" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="270" x14ac:dyDescent="0.25">
@@ -2170,7 +2170,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>41</v>
@@ -2179,7 +2179,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>32</v>
@@ -2187,10 +2187,10 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="8" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>42</v>
@@ -2200,7 +2200,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="Q7" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="T7" t="s">
         <v>22</v>
@@ -2212,10 +2212,10 @@
         <v>33</v>
       </c>
       <c r="W7" t="s">
-        <v>260</v>
+        <v>368</v>
       </c>
       <c r="X7" s="13" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="213.75" x14ac:dyDescent="0.25">
@@ -2223,7 +2223,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>44</v>
@@ -2232,7 +2232,7 @@
         <v>45</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>32</v>
@@ -2240,13 +2240,13 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="8" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="J8" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="8"/>
@@ -2254,7 +2254,7 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -2268,13 +2268,13 @@
         <v>33</v>
       </c>
       <c r="W8" t="s">
-        <v>262</v>
+        <v>370</v>
       </c>
       <c r="AA8" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="AB8" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2282,7 +2282,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>48</v>
@@ -2291,7 +2291,7 @@
         <v>49</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>32</v>
@@ -2299,7 +2299,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="8" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>43</v>
@@ -2331,7 +2331,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>50</v>
@@ -2340,7 +2340,7 @@
         <v>51</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>52</v>
@@ -2378,7 +2378,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>53</v>
@@ -2387,7 +2387,7 @@
         <v>54</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>21</v>
@@ -2425,7 +2425,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>55</v>
@@ -2434,7 +2434,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>32</v>
@@ -2442,13 +2442,13 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="8" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="J12" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="8"/>
@@ -2456,7 +2456,7 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
@@ -2470,13 +2470,13 @@
         <v>33</v>
       </c>
       <c r="W12" t="s">
-        <v>263</v>
+        <v>371</v>
       </c>
       <c r="AA12" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="AB12" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
@@ -2484,7 +2484,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>57</v>
@@ -2493,7 +2493,7 @@
         <v>58</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>32</v>
@@ -2501,13 +2501,13 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="8" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="J13" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="8"/>
@@ -2515,7 +2515,7 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="11" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
@@ -2529,13 +2529,13 @@
         <v>33</v>
       </c>
       <c r="W13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="Y13" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AA13" s="13" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>59</v>
@@ -2552,7 +2552,7 @@
         <v>60</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>32</v>
@@ -2560,7 +2560,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="8" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>43</v>
@@ -2592,7 +2592,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>61</v>
@@ -2609,7 +2609,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="8" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>43</v>
@@ -2641,7 +2641,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>63</v>
@@ -2661,10 +2661,10 @@
       <c r="H16" s="3"/>
       <c r="I16" s="8"/>
       <c r="J16" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="K16" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="8"/>
@@ -2684,7 +2684,7 @@
         <v>29</v>
       </c>
       <c r="W16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>66</v>
@@ -2709,13 +2709,13 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="8" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="J17" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="K17" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="8"/>
@@ -2735,16 +2735,16 @@
         <v>29</v>
       </c>
       <c r="W17" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="X17" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="Y17" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="AA17" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
@@ -2752,7 +2752,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>68</v>
@@ -2772,10 +2772,10 @@
       <c r="H18" s="3"/>
       <c r="I18" s="8"/>
       <c r="J18" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="K18" s="11" t="s">
         <v>238</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="8"/>
@@ -2795,7 +2795,7 @@
         <v>29</v>
       </c>
       <c r="W18" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
@@ -2803,7 +2803,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>71</v>
@@ -2820,13 +2820,13 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="8" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="J19" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="K19" s="11" t="s">
         <v>238</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="8"/>
@@ -2846,16 +2846,16 @@
         <v>29</v>
       </c>
       <c r="W19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="X19" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="Y19" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="AA19" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
@@ -2863,7 +2863,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>73</v>
@@ -2883,10 +2883,10 @@
       <c r="H20" s="3"/>
       <c r="I20" s="8"/>
       <c r="J20" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="8"/>
@@ -2906,7 +2906,7 @@
         <v>29</v>
       </c>
       <c r="W20" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
@@ -2914,7 +2914,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>76</v>
@@ -2963,7 +2963,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>78</v>
@@ -2980,7 +2980,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="8" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>43</v>
@@ -3012,7 +3012,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>80</v>
@@ -3061,7 +3061,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>83</v>
@@ -3104,7 +3104,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>85</v>
@@ -3113,7 +3113,7 @@
         <v>86</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>32</v>
@@ -3153,7 +3153,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>88</v>
@@ -3162,7 +3162,7 @@
         <v>89</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>32</v>
@@ -3202,7 +3202,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>90</v>
@@ -3251,7 +3251,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>93</v>
@@ -3300,7 +3300,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>96</v>
@@ -3317,7 +3317,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="8" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="J29" s="11" t="s">
         <v>43</v>
@@ -3349,7 +3349,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>98</v>
@@ -3398,7 +3398,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>101</v>
@@ -3447,7 +3447,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>104</v>
@@ -3496,7 +3496,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>107</v>
@@ -3545,7 +3545,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>109</v>
@@ -3594,7 +3594,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>111</v>
@@ -3643,7 +3643,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>113</v>
@@ -3692,7 +3692,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>115</v>
@@ -3741,7 +3741,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>118</v>
@@ -3750,7 +3750,7 @@
         <v>119</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>52</v>
@@ -3790,7 +3790,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>122</v>
@@ -3799,7 +3799,7 @@
         <v>123</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>32</v>
@@ -3807,13 +3807,13 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="8" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="J39" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="K39" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>242</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="8"/>
@@ -3821,7 +3821,7 @@
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
       <c r="Q39" s="11" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
@@ -3835,7 +3835,7 @@
         <v>33</v>
       </c>
       <c r="W39" t="s">
-        <v>267</v>
+        <v>376</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
@@ -3843,7 +3843,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>124</v>
@@ -3852,7 +3852,7 @@
         <v>125</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>52</v>
@@ -3891,7 +3891,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>126</v>
@@ -3900,7 +3900,7 @@
         <v>127</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>32</v>
@@ -3908,13 +3908,13 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="8" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="8"/>
@@ -3922,7 +3922,7 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="11" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="R41" s="3"/>
       <c r="S41" s="11"/>
@@ -3936,7 +3936,7 @@
         <v>159</v>
       </c>
       <c r="W41" s="13" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
@@ -3944,7 +3944,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>128</v>
@@ -3993,7 +3993,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>131</v>
@@ -4002,7 +4002,7 @@
         <v>132</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>52</v>
@@ -4013,10 +4013,10 @@
       <c r="H43" s="3"/>
       <c r="I43" s="8"/>
       <c r="J43" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="K43" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>244</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="8"/>
@@ -4036,16 +4036,16 @@
         <v>29</v>
       </c>
       <c r="W43" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="Y43" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="AA43" s="13" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="AB43" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="44" spans="1:28" ht="51" x14ac:dyDescent="0.25">
@@ -4053,7 +4053,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>134</v>
@@ -4070,7 +4070,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="8" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="J44" s="11" t="s">
         <v>43</v>
@@ -4102,7 +4102,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>136</v>
@@ -4111,7 +4111,7 @@
         <v>137</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>32</v>
@@ -4119,13 +4119,13 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="8" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="J45" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="8"/>
@@ -4133,7 +4133,7 @@
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
       <c r="Q45" s="11" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
@@ -4147,7 +4147,7 @@
         <v>33</v>
       </c>
       <c r="W45" t="s">
-        <v>270</v>
+        <v>377</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="213.75" x14ac:dyDescent="0.25">
@@ -4155,7 +4155,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>138</v>
@@ -4172,13 +4172,13 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="8" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="J46" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="K46" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="8"/>
@@ -4186,7 +4186,7 @@
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="11" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
@@ -4200,7 +4200,7 @@
         <v>33</v>
       </c>
       <c r="W46" t="s">
-        <v>275</v>
+        <v>378</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.25">
@@ -4208,7 +4208,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>140</v>
@@ -4228,10 +4228,10 @@
       <c r="H47" s="3"/>
       <c r="I47" s="8"/>
       <c r="J47" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="K47" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="8"/>
@@ -4240,7 +4240,7 @@
       <c r="P47" s="3"/>
       <c r="Q47" s="3"/>
       <c r="R47" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S47" s="3"/>
       <c r="T47" t="s">
@@ -4253,7 +4253,7 @@
         <v>29</v>
       </c>
       <c r="W47" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="99.75" x14ac:dyDescent="0.25">
@@ -4261,7 +4261,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>143</v>
@@ -4278,13 +4278,13 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="8" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="J48" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="K48" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="8"/>
@@ -4292,7 +4292,7 @@
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="11" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
@@ -4306,7 +4306,7 @@
         <v>33</v>
       </c>
       <c r="W48" t="s">
-        <v>220</v>
+        <v>379</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
@@ -4314,7 +4314,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>145</v>
@@ -4323,7 +4323,7 @@
         <v>146</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>32</v>
@@ -4331,7 +4331,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J49" s="11" t="s">
         <v>43</v>
@@ -4362,7 +4362,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>147</v>
@@ -4371,7 +4371,7 @@
         <v>148</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>32</v>
@@ -4379,7 +4379,7 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>43</v>
@@ -4411,7 +4411,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>149</v>
@@ -4428,7 +4428,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J51" s="11" t="s">
         <v>43</v>
@@ -4460,7 +4460,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>151</v>
@@ -4477,7 +4477,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="8" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="J52" s="11" t="s">
         <v>43</v>
@@ -4509,7 +4509,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>153</v>
@@ -4526,7 +4526,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J53" s="11" t="s">
         <v>43</v>
@@ -4558,7 +4558,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>155</v>
@@ -4575,7 +4575,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J54" s="11" t="s">
         <v>43</v>
@@ -4607,7 +4607,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>157</v>
@@ -4624,7 +4624,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J55" s="11" t="s">
         <v>43</v>
@@ -4651,10 +4651,10 @@
         <v>46</v>
       </c>
       <c r="AA55" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="AB55" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
@@ -4662,7 +4662,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>160</v>
@@ -4679,7 +4679,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J56" s="11" t="s">
         <v>43</v>
@@ -4711,7 +4711,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>162</v>
@@ -4728,7 +4728,7 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J57" s="11" t="s">
         <v>43</v>
@@ -4755,10 +4755,10 @@
         <v>46</v>
       </c>
       <c r="AA57" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="AB57" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58" spans="1:28" ht="28.5" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>164</v>
@@ -4775,7 +4775,7 @@
         <v>165</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>32</v>
@@ -4783,10 +4783,10 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K58" s="3" t="s">
         <v>165</v>
@@ -4797,7 +4797,7 @@
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
       <c r="Q58" s="11" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
@@ -4814,10 +4814,10 @@
         <v>46</v>
       </c>
       <c r="Y58" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="AA58" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.25">
@@ -4825,7 +4825,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>166</v>
@@ -4872,7 +4872,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>168</v>
@@ -4919,7 +4919,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>170</v>
@@ -4966,7 +4966,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>172</v>
@@ -5013,7 +5013,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>174</v>
@@ -5060,7 +5060,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>176</v>
@@ -5107,7 +5107,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>178</v>
@@ -5154,7 +5154,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>180</v>
@@ -5171,7 +5171,7 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="8" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="J66" s="11" t="s">
         <v>43</v>
@@ -5203,7 +5203,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>182</v>
@@ -5252,7 +5252,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>185</v>
@@ -5269,7 +5269,7 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="8" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="J68" s="11" t="s">
         <v>43</v>
@@ -5301,7 +5301,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>187</v>
@@ -5318,13 +5318,13 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="8" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="J69" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="K69" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="L69" s="3"/>
       <c r="M69" s="8"/>
@@ -5332,7 +5332,7 @@
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="R69" s="3"/>
       <c r="S69" s="3"/>
@@ -5346,7 +5346,7 @@
         <v>33</v>
       </c>
       <c r="W69" t="s">
-        <v>274</v>
+        <v>380</v>
       </c>
     </row>
     <row r="70" spans="1:24" ht="51" x14ac:dyDescent="0.25">
@@ -5354,7 +5354,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>189</v>
@@ -5371,7 +5371,7 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="8" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="J70" s="11" t="s">
         <v>43</v>
@@ -5403,7 +5403,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>191</v>
@@ -5420,7 +5420,7 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="8" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="J71" s="11" t="s">
         <v>43</v>
@@ -5452,7 +5452,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>193</v>
@@ -5469,7 +5469,7 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="8" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="J72" s="11" t="s">
         <v>43</v>
@@ -5501,7 +5501,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>195</v>
@@ -5510,7 +5510,7 @@
         <v>196</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>32</v>
@@ -5518,7 +5518,7 @@
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="8" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="J73" s="11" t="s">
         <v>43</v>
@@ -5550,7 +5550,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>197</v>
@@ -5559,7 +5559,7 @@
         <v>198</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>32</v>
@@ -5567,7 +5567,7 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="8" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="J74" s="11" t="s">
         <v>43</v>
@@ -5599,7 +5599,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>199</v>
@@ -5608,7 +5608,7 @@
         <v>200</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>32</v>
@@ -5616,7 +5616,7 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="8" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="J75" s="11" t="s">
         <v>43</v>
@@ -5648,7 +5648,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>201</v>
@@ -5657,7 +5657,7 @@
         <v>202</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>32</v>
@@ -5697,7 +5697,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>203</v>
@@ -5706,14 +5706,14 @@
         <v>204</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G77" s="3"/>
       <c r="I77" s="9" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="J77" s="11" t="s">
         <v>43</v>
@@ -5745,7 +5745,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>205</v>
@@ -5754,7 +5754,7 @@
         <v>206</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>32</v>
@@ -5762,7 +5762,7 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="8" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="J78" s="11" t="s">
         <v>43</v>
@@ -5794,7 +5794,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>207</v>
@@ -5811,7 +5811,7 @@
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="8" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="J79" s="11" t="s">
         <v>43</v>
@@ -5838,7 +5838,7 @@
         <v>46</v>
       </c>
       <c r="X79" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="80" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -5846,7 +5846,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>209</v>
@@ -5855,7 +5855,7 @@
         <v>210</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>32</v>
@@ -5863,7 +5863,7 @@
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J80" s="11" t="s">
         <v>43</v>
@@ -5895,7 +5895,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>211</v>
@@ -5904,7 +5904,7 @@
         <v>212</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>32</v>
@@ -5912,7 +5912,7 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J81" s="11" t="s">
         <v>43</v>
@@ -5944,7 +5944,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>213</v>
@@ -5953,7 +5953,7 @@
         <v>214</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>32</v>
@@ -5961,7 +5961,7 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="J82" s="11" t="s">
         <v>43</v>
@@ -5969,7 +5969,7 @@
       <c r="K82" s="11"/>
       <c r="L82" s="11"/>
       <c r="M82" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N82" s="11"/>
       <c r="O82" s="3"/>
@@ -5990,10 +5990,10 @@
         <v>46</v>
       </c>
       <c r="X82" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="AA82" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.25">
@@ -6001,7 +6001,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>215</v>
@@ -6010,7 +6010,7 @@
         <v>216</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>32</v>
@@ -6048,7 +6048,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>217</v>
@@ -6057,7 +6057,7 @@
         <v>218</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
add admin date variable
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9FA8E8-0C19-4A03-BC72-D25922AC7553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E0CE3C-D2BE-47C7-A6C7-14F4E3D5B154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="383">
   <si>
     <t>index</t>
   </si>
@@ -1314,6 +1314,12 @@
   </si>
   <si>
     <t>recode("No"=0; "Yes, slightly troubled"=1; "Yes, very troubled"=1; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>besvardato</t>
+  </si>
+  <si>
+    <t>as.Date(besvardato,format="%d %b %y")</t>
   </si>
 </sst>
 </file>
@@ -1455,7 +1461,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1774,13 +1780,13 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T7" sqref="T7"/>
+      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="2" customWidth="1"/>
@@ -1973,7 +1979,7 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="11" t="s">
-        <v>43</v>
+        <v>381</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1985,16 +1991,16 @@
       <c r="R3" s="3"/>
       <c r="S3" s="11"/>
       <c r="T3" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="U3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="V3" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="W3" t="s">
-        <v>46</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correct warning for bmi, sp48a and drukuge2
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E0CE3C-D2BE-47C7-A6C7-14F4E3D5B154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8EDF4D-215D-4F00-AEE1-9840421B0B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -1268,15 +1268,6 @@
     <t>Number of non-missing items in the SF36 physical function subscale</t>
   </si>
   <si>
-    <t>as.numeric(bmi)</t>
-  </si>
-  <si>
-    <t>as.numeric(drukuge2)*12</t>
-  </si>
-  <si>
-    <t>as.numeric(sp28a)*7</t>
-  </si>
-  <si>
     <t>recode("Danish ethnicity"=1; "Western ethnicity" =1; ELSE=NA)</t>
   </si>
   <si>
@@ -1320,6 +1311,15 @@
   </si>
   <si>
     <t>as.Date(besvardato,format="%d %b %y")</t>
+  </si>
+  <si>
+    <t>ifelse(bmi == "irrelevant,NA,as.numeric(bmi))</t>
+  </si>
+  <si>
+    <t>ifelse(drukuge2 == "irrelevant,NA,as.numeric(drukuge2))*12</t>
+  </si>
+  <si>
+    <t>ifelse(sp28a == "irrelevant,NA,as.numeric(sp28a))*7</t>
   </si>
 </sst>
 </file>
@@ -1780,37 +1780,37 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomRight" activeCell="W46" sqref="W46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="8.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="31.85546875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="21.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" style="2" customWidth="1"/>
-    <col min="23" max="23" width="52.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="2"/>
+    <col min="8" max="8" width="8.54296875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="36.7265625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="25.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="30.1796875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="31.81640625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="7.7265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.26953125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="12.7265625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.54296875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="19.81640625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="52.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="11" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -2000,10 +2000,10 @@
         <v>29</v>
       </c>
       <c r="W3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="25" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2053,10 +2053,10 @@
         <v>33</v>
       </c>
       <c r="W4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="168" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="270" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="232" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2218,13 +2218,13 @@
         <v>33</v>
       </c>
       <c r="W7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="X7" s="13" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="196" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>33</v>
       </c>
       <c r="W8" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="AA8" t="s">
         <v>294</v>
@@ -2283,7 +2283,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="25" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="196" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>33</v>
       </c>
       <c r="W12" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="AA12" t="s">
         <v>302</v>
@@ -2485,7 +2485,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="25" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="25" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2690,10 +2690,10 @@
         <v>29</v>
       </c>
       <c r="W16" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="25" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>29</v>
       </c>
       <c r="W17" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="X17" t="s">
         <v>311</v>
@@ -2753,7 +2753,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2801,10 +2801,10 @@
         <v>29</v>
       </c>
       <c r="W18" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="25" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>29</v>
       </c>
       <c r="W19" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="X19" t="s">
         <v>311</v>
@@ -2864,7 +2864,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2912,10 +2912,10 @@
         <v>29</v>
       </c>
       <c r="W20" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="25" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="228" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="182" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3841,10 +3841,10 @@
         <v>33</v>
       </c>
       <c r="W39" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="171" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="168" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="300" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>29</v>
       </c>
       <c r="W43" t="s">
-        <v>366</v>
+        <v>381</v>
       </c>
       <c r="Y43" t="s">
         <v>326</v>
@@ -4054,7 +4054,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="51" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="50" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="210" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4153,10 +4153,10 @@
         <v>33</v>
       </c>
       <c r="W45" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" ht="213.75" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" ht="210" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4206,10 +4206,10 @@
         <v>33</v>
       </c>
       <c r="W46" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4259,10 +4259,10 @@
         <v>29</v>
       </c>
       <c r="W47" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28" ht="99.75" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" ht="98" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4312,10 +4312,10 @@
         <v>33</v>
       </c>
       <c r="W48" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="49" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" ht="25" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="25" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="25" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="25" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" ht="25" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" ht="25" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" ht="25" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" ht="25" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="28" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="50" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:24" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="98" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -5352,10 +5352,10 @@
         <v>33</v>
       </c>
       <c r="W69" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" ht="50" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="50" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="50" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="137.5" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:24" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="76" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="80" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" ht="25" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" ht="25" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="102" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" ht="100" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Correct bmi, alcohol, smoking
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41CC4FB-0B18-4207-BB72-013D480E299A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58A02F7-0A3A-4701-91AE-30E993AE52EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1313,13 +1313,13 @@
     <t>as.Date(besvardato,format="%d %b %y")</t>
   </si>
   <si>
-    <t>ifelse(bmi %in%  c("irrelevant","Uoplyst") | is.na(bmi),NA,as.numeric(bmi))</t>
-  </si>
-  <si>
-    <t>ifelse(drukuge2 %in%  c("irrelevant","Uoplyst") | is.na(drukuge2),NA,as.numeric(drukuge2))*12</t>
-  </si>
-  <si>
-    <t>ifelse(sp28a %in%  c("irrelevant","Uoplyst") | is.na(sp28a),NA,as.numeric(sp28a))*7</t>
+    <t>ifelse(bmi %in%  c("irrelevant","Uoplyst",".") | is.na(bmi),NA,as.numeric(bmi))</t>
+  </si>
+  <si>
+    <t>ifelse(sp28a %in%  c("irrelevant","Uoplyst",".") | is.na(sp28a),NA,as.numeric(sp28a)*7)</t>
+  </si>
+  <si>
+    <t>ifelse(drukuge2 %in%  c("irrelevant","Uoplyst",".") | is.na(drukuge2),NA,as.numeric(drukuge2)*12)</t>
   </si>
 </sst>
 </file>
@@ -1780,10 +1780,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
+      <selection pane="bottomRight" activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4042,7 +4042,7 @@
         <v>29</v>
       </c>
       <c r="W43" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="Y43" t="s">
         <v>326</v>
@@ -4259,7 +4259,7 @@
         <v>29</v>
       </c>
       <c r="W47" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="98" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
correct bmi, alcohol and smoking again
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58A02F7-0A3A-4701-91AE-30E993AE52EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA59414-C6D4-4AF3-965F-E9A86809E309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1313,13 +1313,13 @@
     <t>as.Date(besvardato,format="%d %b %y")</t>
   </si>
   <si>
-    <t>ifelse(bmi %in%  c("irrelevant","Uoplyst",".") | is.na(bmi),NA,as.numeric(bmi))</t>
-  </si>
-  <si>
-    <t>ifelse(sp28a %in%  c("irrelevant","Uoplyst",".") | is.na(sp28a),NA,as.numeric(sp28a)*7)</t>
-  </si>
-  <si>
-    <t>ifelse(drukuge2 %in%  c("irrelevant","Uoplyst",".") | is.na(drukuge2),NA,as.numeric(drukuge2)*12)</t>
+    <t>ifelse(bmi %in%  c("irrelevant","Irrelevant","Uoplyst",".",".u") | is.na(bmi),NA,as.numeric(bmi))</t>
+  </si>
+  <si>
+    <t>ifelse(drukuge2 %in%  c("irrelevant","Irrelevant","Uoplyst",".",".u") | is.na(drukuge2),NA,as.numeric(drukuge2)*12)</t>
+  </si>
+  <si>
+    <t>ifelse(sp28a %in%  c("irrelevant","Irrelevant","Uoplyst",".",".u") | is.na(sp28a),NA,as.numeric(sp28a)*7)</t>
   </si>
 </sst>
 </file>
@@ -1783,7 +1783,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="S13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W16" sqref="W16"/>
+      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4042,7 +4042,7 @@
         <v>29</v>
       </c>
       <c r="W43" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Y43" t="s">
         <v>326</v>
@@ -4259,7 +4259,7 @@
         <v>29</v>
       </c>
       <c r="W47" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="98" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
correct date harmo rule
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA59414-C6D4-4AF3-965F-E9A86809E309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C77BDC5-E6AD-4216-A1EA-C2756B6FFAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -1310,9 +1310,6 @@
     <t>besvardato</t>
   </si>
   <si>
-    <t>as.Date(besvardato,format="%d %b %y")</t>
-  </si>
-  <si>
     <t>ifelse(bmi %in%  c("irrelevant","Irrelevant","Uoplyst",".",".u") | is.na(bmi),NA,as.numeric(bmi))</t>
   </si>
   <si>
@@ -1320,6 +1317,9 @@
   </si>
   <si>
     <t>ifelse(sp28a %in%  c("irrelevant","Irrelevant","Uoplyst",".",".u") | is.na(sp28a),NA,as.numeric(sp28a)*7)</t>
+  </si>
+  <si>
+    <t>ifelse(grepl("-",besvardato),as.Date(besvardato, format = "%d-%b-%y"),as.Date(besvardato, format = "%d%b%Y"))</t>
   </si>
 </sst>
 </file>
@@ -1780,37 +1780,38 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
+      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="2"/>
-    <col min="8" max="8" width="8.54296875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="36.7265625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="25.1796875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26.453125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="30.1796875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="31.81640625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="7.7265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="21.26953125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="12.7265625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12.453125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="17.54296875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="19.81640625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="52.7265625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="8.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="31.85546875" style="9" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="19.85546875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="124" customWidth="1"/>
+    <col min="24" max="24" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1954,7 +1955,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2000,10 +2001,10 @@
         <v>29</v>
       </c>
       <c r="W3" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" ht="25" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2056,7 +2057,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2115,7 +2116,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="168" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="232" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="270" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2224,7 +2225,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="196" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2379,7 +2380,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2426,7 +2427,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="196" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2544,7 +2545,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2593,7 +2594,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2642,7 +2643,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2693,7 +2694,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2864,7 +2865,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2912,10 +2913,10 @@
         <v>29</v>
       </c>
       <c r="W20" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2964,7 +2965,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3013,7 +3014,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3062,7 +3063,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3105,7 +3106,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3203,7 +3204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3301,7 +3302,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3350,7 +3351,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3399,7 +3400,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3448,7 +3449,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3497,7 +3498,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3546,7 +3547,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3595,7 +3596,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3644,7 +3645,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3693,7 +3694,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3742,7 +3743,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3791,7 +3792,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="182" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" ht="228" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3844,7 +3845,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3892,7 +3893,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="168" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" ht="171" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3945,7 +3946,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3994,7 +3995,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" ht="330" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -4042,7 +4043,7 @@
         <v>29</v>
       </c>
       <c r="W43" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="Y43" t="s">
         <v>326</v>
@@ -4054,7 +4055,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="50" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -4103,7 +4104,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="210" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4156,7 +4157,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="210" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4209,7 +4210,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4259,10 +4260,10 @@
         <v>29</v>
       </c>
       <c r="W47" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28" ht="98" x14ac:dyDescent="0.35">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4315,7 +4316,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="25" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4363,7 +4364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="25" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4412,7 +4413,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="25" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4461,7 +4462,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4510,7 +4511,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -4559,7 +4560,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4608,7 +4609,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="25" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4663,7 +4664,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="25" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4712,7 +4713,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4767,7 +4768,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="28" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4826,7 +4827,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4873,7 +4874,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4920,7 +4921,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4967,7 +4968,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -5014,7 +5015,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -5061,7 +5062,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -5108,7 +5109,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -5155,7 +5156,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="50" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -5204,7 +5205,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -5253,7 +5254,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:24" ht="112.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5302,7 +5303,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:24" ht="98" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -5355,7 +5356,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="70" spans="1:24" ht="50" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5404,7 +5405,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:24" ht="50" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -5453,7 +5454,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:24" ht="50" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -5502,7 +5503,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:24" ht="137.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -5551,7 +5552,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -5600,7 +5601,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -5649,7 +5650,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -5698,7 +5699,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:24" ht="76" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:24" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -5746,7 +5747,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -5795,7 +5796,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:24" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -5847,7 +5848,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="80" spans="1:24" ht="25" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -5896,7 +5897,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:27" ht="25" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -5945,7 +5946,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="100" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:27" ht="102" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -6002,7 +6003,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -6049,7 +6050,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
correct date harmo rule to avoid valuetype error
</commit_message>
<xml_diff>
--- a/data_processing_elements-DNH.xlsx
+++ b/data_processing_elements-DNH.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C77BDC5-E6AD-4216-A1EA-C2756B6FFAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7538DA5-E8B8-4F1E-9540-2832ECB50C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1319,14 +1319,14 @@
     <t>ifelse(sp28a %in%  c("irrelevant","Irrelevant","Uoplyst",".",".u") | is.na(sp28a),NA,as.numeric(sp28a)*7)</t>
   </si>
   <si>
-    <t>ifelse(grepl("-",besvardato),as.Date(besvardato, format = "%d-%b-%y"),as.Date(besvardato, format = "%d%b%Y"))</t>
+    <t>ifelse(grepl("-",besvardato),as.character(as.Date(besvardato, format = "%d-%b-%y")),as.character(as.Date(besvardato, format = "%d%b%Y")))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1357,6 +1357,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1399,7 +1405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1438,6 +1444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2000,7 +2007,7 @@
       <c r="V3" t="s">
         <v>29</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="14" t="s">
         <v>382</v>
       </c>
     </row>
@@ -3995,7 +4002,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="330" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="300" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>

</xml_diff>